<commit_message>
add device name column to reports
</commit_message>
<xml_diff>
--- a/templates/export/route.xlsx
+++ b/templates/export/route.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Автор</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -32,13 +27,12 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="H9")</t>
+          <t>jx:area(lastCell="I9")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,23 +40,22 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="204"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="H9" multisheet="sheetNames")</t>
+          <t>jx:each(items="devices", var="device", lastCell="I9" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0">
+    <comment ref="A9" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
+            <charset val="1"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="position", lastCell="H9")</t>
+          <t>jx:each(items="device.objects", var="position", lastCell="I9")</t>
         </r>
       </text>
     </comment>
@@ -71,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Report type:</t>
   </si>
@@ -143,18 +136,24 @@
   </si>
   <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", position.fixTime, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>Device Name</t>
+  </si>
+  <si>
+    <t>${position.deviceName}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0&quot; m&quot;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -233,14 +232,13 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
-      <color rgb="FF000000"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -253,7 +251,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF5B9BD5"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -342,69 +340,69 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Пояснение" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF5B9BD5"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0070C0"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF444444"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="005B9BD5"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000070C0"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00444444"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
       <rgbColor rgb="00003366"/>
       <rgbColor rgb="00339966"/>
       <rgbColor rgb="00003300"/>
@@ -449,7 +447,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11381760" cy="9524520"/>
+          <a:ext cx="9525000" cy="9525000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -461,20 +459,22 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:miter/>
+          <a:miter lim="800000"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:effectRef>
-        <a:fontRef idx="minor"/>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
       </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
@@ -500,7 +500,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11381760" cy="9524520"/>
+          <a:ext cx="9525000" cy="9525000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -512,20 +512,22 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:miter/>
+          <a:miter lim="800000"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:effectRef>
-        <a:fontRef idx="minor"/>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
       </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
@@ -551,7 +553,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11381760" cy="9524520"/>
+          <a:ext cx="9525000" cy="9525000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -563,20 +565,22 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:miter/>
+          <a:miter lim="800000"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:effectRef>
-        <a:fontRef idx="minor"/>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
       </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
@@ -617,10 +621,15 @@
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
         </a:ln>
       </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -660,10 +669,15 @@
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
         </a:ln>
       </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -703,10 +717,15 @@
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
         </a:ln>
       </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -756,7 +775,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -791,7 +810,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -968,33 +987,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375"/>
-    <col min="2" max="2" width="20.7109375"/>
-    <col min="3" max="4" width="13"/>
-    <col min="5" max="5" width="10.7109375"/>
-    <col min="6" max="6" width="11.42578125"/>
-    <col min="7" max="7" width="61.85546875"/>
-    <col min="8" max="8" width="73.28515625"/>
-    <col min="9" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="61.88671875" customWidth="1"/>
+    <col min="8" max="8" width="73.33203125" customWidth="1"/>
+    <col min="9" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1004,7 +1023,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1037,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1028,7 +1047,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1042,7 +1061,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1056,7 +1075,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1089,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="8"/>
@@ -1080,61 +1099,67 @@
       <c r="G7" s="8"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="29.25" customHeight="1">
       <c r="A8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="19" customFormat="1" ht="18.75" customHeight="1">
       <c r="A9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="F9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="G9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="I9" s="18" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>